<commit_message>
30. Add: Função SE
</commit_message>
<xml_diff>
--- a/04 - Logica Booleana e Buscas de Valores.xlsx
+++ b/04 - Logica Booleana e Buscas de Valores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Dev\Cursos\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9DA03-7CD1-4D49-8B29-C5DBF05D7E71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7CD14C-8C3A-46A7-8F6A-95DD81C05F8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="23070" windowHeight="12195" tabRatio="698" activeTab="4" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="23070" windowHeight="12195" tabRatio="698" activeTab="4" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="25" r:id="rId1"/>
@@ -613,10 +613,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -1298,7 +1299,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1600,6 +1601,9 @@
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -8843,7 +8847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ADA2D8-DE9E-4ACF-B5A7-8907124C5CF1}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -12653,7 +12657,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" zeroHeight="1"/>
@@ -12714,7 +12718,7 @@
         <v>155</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E6" s="73" t="s">
         <v>160</v>
@@ -12729,13 +12733,13 @@
       </c>
       <c r="C7" s="50" t="str">
         <f>IFERROR(VLOOKUP(C6,TB_Produtos[#All],2,FALSE),"Não encontrado")</f>
-        <v>Bermuda</v>
+        <v>Calça jeans</v>
       </c>
       <c r="E7" s="73" t="s">
         <v>163</v>
       </c>
       <c r="F7" s="50" t="str">
-        <f>HLOOKUP(WEEKDAY(F6),'Cadastros Auxiliares'!B4:I5,2,FALSE)</f>
+        <f>IFERROR(HLOOKUP(WEEKDAY(F6),'Cadastros Auxiliares'!B4:I5,2,FALSE),"")</f>
         <v>Sábado</v>
       </c>
       <c r="G7" s="49"/>
@@ -12746,7 +12750,7 @@
       </c>
       <c r="C8" s="48" t="str">
         <f>IFERROR(VLOOKUP(C6,TB_Produtos[#All],3,FALSE),"Não encontrado")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E8" s="74" t="s">
         <v>164</v>
@@ -12775,9 +12779,9 @@
       <c r="B10" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="118">
         <f>IFERROR(VLOOKUP($C$6,Produtos!$B$6:$G$66,6,0),"Não encontrado")</f>
-        <v>69.900000000000006</v>
+        <v>85.9</v>
       </c>
       <c r="G10" s="49"/>
     </row>
@@ -12785,7 +12789,10 @@
       <c r="B11" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="C11" s="48"/>
+      <c r="C11" s="48">
+        <f>VLOOKUP(C6,TB_Produtos[#All],5,FALSE)</f>
+        <v>24</v>
+      </c>
       <c r="F11" t="s">
         <v>169</v>
       </c>
@@ -12795,7 +12802,10 @@
       <c r="B12" s="79" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="48"/>
+      <c r="C12" s="118" t="str">
+        <f>IF(C11&gt;10,"Estoque OK", IF(C11=0,"Estoque zerado", "Rever estoque"))</f>
+        <v>Estoque OK</v>
+      </c>
       <c r="E12" s="80"/>
       <c r="F12" t="s">
         <v>170</v>

</xml_diff>